<commit_message>
Debugging Session4 from previous session(TBC)
</commit_message>
<xml_diff>
--- a/List.xlsx
+++ b/List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\VSCode Projects\pool-cost-calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECB19CC2-78F0-4AB0-9033-5B68D4D6707E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2193DA-9AB6-4E27-BB4C-2B3724A843AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-7215" windowWidth="16440" windowHeight="28320" xr2:uid="{BE88EEF3-4FF8-43A6-B5B5-5525606DC647}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="9">
   <si>
     <t>H</t>
   </si>
@@ -58,6 +58,12 @@
   <si>
     <t>K</t>
   </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
 </sst>
 </file>
 
@@ -72,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -82,6 +88,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -150,20 +162,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -171,6 +177,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -507,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9C6144-6401-498D-8D34-6B35F906CB82}">
-  <dimension ref="B2:F82"/>
+  <dimension ref="B2:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,23 +540,29 @@
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="2">
+      <c r="C2" s="9">
         <v>45795</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="H2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -543,15 +571,23 @@
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="5">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -560,15 +596,23 @@
       <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="5">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="H4" s="4"/>
+      <c r="I4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -577,9 +621,17 @@
       <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="5">
+      <c r="H5" s="4"/>
+      <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -588,334 +640,576 @@
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="2">
+      <c r="E6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" s="9">
         <v>45802</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="5">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="5">
-        <v>3</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="5">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="5">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="5">
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="H7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="13"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
         <v>6</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="5">
+      <c r="C13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
         <v>7</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="5">
+      <c r="C14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
         <v>8</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-      <c r="C16" s="2">
+      <c r="C15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="9">
         <v>45802</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="6">
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="H16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
         <v>1</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="4" t="s">
+      <c r="D17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="6">
+      <c r="H17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
         <v>2</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="D18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
-      <c r="C19" s="2">
+      <c r="H18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="9">
         <v>45809</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="5">
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="H19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
         <v>1</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="5">
+      <c r="H20" s="4"/>
+      <c r="I20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
         <v>2</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="5">
+      <c r="H21" s="4"/>
+      <c r="I21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
         <v>3</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="5">
+      <c r="H22" s="4"/>
+      <c r="I22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
         <v>4</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="5">
+      <c r="H23" s="4"/>
+      <c r="I23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
         <v>5</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="5">
+      <c r="H24" s="4"/>
+      <c r="I24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
         <v>6</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="5">
+      <c r="H25" s="4"/>
+      <c r="I25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
         <v>7</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="5">
+      <c r="H26" s="4"/>
+      <c r="I26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
         <v>8</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="D27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="5">
+      <c r="H27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="3">
         <v>9</v>
       </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="5"/>
-      <c r="C29" s="7">
+      <c r="H28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K28" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="5">
         <v>45814</v>
       </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="9"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="5">
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7"/>
+      <c r="H29" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="3">
         <v>1</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -923,49 +1217,49 @@
       </c>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="5">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="3">
         <v>2</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="5">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="3">
         <v>3</v>
       </c>
       <c r="C32" s="1"/>
-      <c r="D32" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="D32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="5"/>
-      <c r="C33" s="7">
+      <c r="B33" s="3"/>
+      <c r="C33" s="5">
         <v>45814</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="9"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="7"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="5">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" s="3" t="s">
+      <c r="B34" s="3">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="1" t="s">
@@ -976,13 +1270,13 @@
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="5">
-        <v>2</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" s="3" t="s">
+      <c r="B35" s="3">
+        <v>2</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E35" s="1" t="s">
@@ -993,13 +1287,13 @@
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="5">
-        <v>3</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" s="3" t="s">
+      <c r="B36" s="3">
+        <v>3</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E36" s="1" t="s">
@@ -1010,276 +1304,276 @@
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="5">
+      <c r="B37" s="3">
         <v>4</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F37" s="3" t="s">
+      <c r="D37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="5"/>
-      <c r="C38" s="2">
+      <c r="B38" s="3"/>
+      <c r="C38" s="9">
         <v>45814</v>
       </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="5">
+      <c r="B39" s="3">
         <v>1</v>
       </c>
       <c r="C39" s="1"/>
-      <c r="D39" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E39" s="3" t="s">
+      <c r="D39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="5">
+      <c r="B40" s="3">
         <v>2</v>
       </c>
       <c r="C40" s="1"/>
-      <c r="D40" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E40" s="3" t="s">
+      <c r="D40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="5">
+      <c r="B41" s="3">
         <v>3</v>
       </c>
       <c r="C41" s="1"/>
-      <c r="D41" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E41" s="3" t="s">
+      <c r="D41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="5">
+      <c r="B42" s="3">
         <v>4</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E42" s="4" t="s">
+      <c r="D42" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
-      <c r="C43" s="2">
+      <c r="C43" s="9">
         <v>45830</v>
       </c>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="6">
+      <c r="B44" s="3">
         <v>1</v>
       </c>
       <c r="C44" s="1"/>
-      <c r="D44" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E44" s="4" t="s">
+      <c r="D44" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="6">
+      <c r="B45" s="3">
         <v>2</v>
       </c>
       <c r="C45" s="1"/>
-      <c r="D45" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E45" s="4" t="s">
+      <c r="D45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="6">
+      <c r="B46" s="3">
         <v>3</v>
       </c>
       <c r="C46" s="1"/>
-      <c r="D46" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E46" s="3" t="s">
+      <c r="D46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="6">
+      <c r="B47" s="3">
         <v>4</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E47" s="4" t="s">
+      <c r="D47" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F47" s="1"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="6">
+      <c r="B48" s="3">
         <v>5</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E48" s="4" t="s">
+      <c r="D48" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="6">
+      <c r="B49" s="3">
         <v>6</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E49" s="4" t="s">
+      <c r="D49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F49" s="1"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="6">
+      <c r="B50" s="3">
         <v>7</v>
       </c>
       <c r="C50" s="1"/>
-      <c r="D50" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E50" s="3" t="s">
+      <c r="D50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F50" s="1"/>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="6">
+      <c r="B51" s="3">
         <v>8</v>
       </c>
       <c r="C51" s="1"/>
-      <c r="D51" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E51" s="4" t="s">
+      <c r="D51" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="6">
+      <c r="B52" s="3">
         <v>9</v>
       </c>
       <c r="C52" s="1"/>
-      <c r="D52" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E52" s="4" t="s">
+      <c r="D52" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="6">
+      <c r="B53" s="3">
         <v>10</v>
       </c>
       <c r="C53" s="1"/>
-      <c r="D53" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E53" s="4" t="s">
+      <c r="D53" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F53" s="1"/>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="6">
+      <c r="B54" s="3">
         <v>11</v>
       </c>
       <c r="C54" s="1"/>
-      <c r="D54" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E54" s="4" t="s">
+      <c r="D54" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="6">
+      <c r="B55" s="3">
         <v>12</v>
       </c>
       <c r="C55" s="1"/>
-      <c r="D55" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E55" s="4" t="s">
+      <c r="D55" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F55" s="1"/>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="6">
+      <c r="B56" s="3">
         <v>13</v>
       </c>
       <c r="C56" s="1"/>
-      <c r="D56" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E56" s="4" t="s">
+      <c r="D56" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
-      <c r="C57" s="2">
+      <c r="C57" s="9">
         <v>45835</v>
       </c>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="6">
+      <c r="B58" s="3">
         <v>1</v>
       </c>
       <c r="C58" s="1"/>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E58" s="1" t="s">
@@ -1288,11 +1582,11 @@
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="6">
+      <c r="B59" s="3">
         <v>2</v>
       </c>
       <c r="C59" s="1"/>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E59" s="1" t="s">
@@ -1301,11 +1595,11 @@
       <c r="F59" s="1"/>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="6">
+      <c r="B60" s="3">
         <v>3</v>
       </c>
       <c r="C60" s="1"/>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E60" s="1" t="s">
@@ -1314,11 +1608,11 @@
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="6">
+      <c r="B61" s="3">
         <v>4</v>
       </c>
       <c r="C61" s="1"/>
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E61" s="1" t="s">
@@ -1327,11 +1621,11 @@
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="6">
+      <c r="B62" s="3">
         <v>5</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E62" s="1" t="s">
@@ -1340,207 +1634,207 @@
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B63" s="6">
+      <c r="B63" s="3">
         <v>6</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E63" s="3" t="s">
+      <c r="D63" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F63" s="1"/>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B64" s="6">
+      <c r="B64" s="3">
         <v>7</v>
       </c>
       <c r="C64" s="1"/>
-      <c r="D64" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E64" s="3" t="s">
+      <c r="D64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F64" s="1"/>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B65" s="6">
+      <c r="B65" s="3">
         <v>8</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E65" s="4" t="s">
+      <c r="D65" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F65" s="1"/>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B66" s="6">
+      <c r="B66" s="3">
         <v>9</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E66" s="3" t="s">
+      <c r="D66" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F66" s="1"/>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B67" s="6">
+      <c r="B67" s="3">
         <v>10</v>
       </c>
       <c r="C67" s="1"/>
-      <c r="D67" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E67" s="3" t="s">
+      <c r="D67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F67" s="1"/>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B68" s="6">
+      <c r="B68" s="3">
         <v>11</v>
       </c>
       <c r="C68" s="1"/>
-      <c r="D68" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E68" s="3" t="s">
+      <c r="D68" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F68" s="1"/>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B69" s="6">
+      <c r="B69" s="3">
         <v>12</v>
       </c>
       <c r="C69" s="1"/>
-      <c r="D69" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E69" s="4" t="s">
+      <c r="D69" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F69" s="1"/>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
-      <c r="C70" s="2">
+      <c r="C70" s="9">
         <v>45838</v>
       </c>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B71" s="6">
+      <c r="B71" s="3">
         <v>1</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E71" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F71" s="1"/>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B72" s="6">
+      <c r="B72" s="3">
         <v>2</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E72" s="3" t="s">
+      <c r="E72" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B73" s="6">
+      <c r="B73" s="3">
         <v>3</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="E73" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F73" s="1"/>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B74" s="6">
+      <c r="B74" s="3">
         <v>4</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="E74" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F74" s="1"/>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B75" s="6">
+      <c r="B75" s="3">
         <v>5</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E75" s="3" t="s">
+      <c r="E75" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F75" s="1"/>
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B76" s="6">
+      <c r="B76" s="3">
         <v>6</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="E76" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F76" s="1"/>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B77" s="6">
+      <c r="B77" s="3">
         <v>7</v>
       </c>
       <c r="C77" s="1"/>
-      <c r="D77" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E77" s="4" t="s">
+      <c r="D77" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F77" s="1"/>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B78" s="5"/>
-      <c r="C78" s="2">
+      <c r="B78" s="3"/>
+      <c r="C78" s="9">
         <v>45838</v>
       </c>
-      <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B79" s="5">
+      <c r="B79" s="3">
         <v>1</v>
       </c>
       <c r="C79" s="1" t="s">
@@ -1549,49 +1843,49 @@
       <c r="D79" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E79" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F79" s="3" t="s">
+      <c r="E79" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F79" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B80" s="6">
-        <v>2</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F80" s="4" t="s">
+      <c r="B80" s="3">
+        <v>2</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F80" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B81" s="5">
-        <v>3</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F81" s="4" t="s">
+      <c r="B81" s="3">
+        <v>3</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F81" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B82" s="6">
+      <c r="B82" s="3">
         <v>4</v>
       </c>
       <c r="C82" s="1" t="s">
@@ -1600,26 +1894,28 @@
       <c r="D82" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E82" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F82" s="3" t="s">
+      <c r="E82" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
     <mergeCell ref="C38:F38"/>
     <mergeCell ref="C43:F43"/>
     <mergeCell ref="C57:F57"/>
     <mergeCell ref="C78:F78"/>
     <mergeCell ref="C70:F70"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="H2:K2"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="H11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Debugging Session5 from previous session(TBC)
</commit_message>
<xml_diff>
--- a/List.xlsx
+++ b/List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\VSCode Projects\pool-cost-calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2193DA-9AB6-4E27-BB4C-2B3724A843AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AE8871-A2AC-4FA5-A704-31DBA091D80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-7215" windowWidth="16440" windowHeight="28320" xr2:uid="{BE88EEF3-4FF8-43A6-B5B5-5525606DC647}"/>
   </bookViews>
@@ -162,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -170,6 +170,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -182,17 +185,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -531,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9C6144-6401-498D-8D34-6B35F906CB82}">
   <dimension ref="B2:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,18 +541,18 @@
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="9">
+      <c r="C2" s="5">
         <v>45795</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="H2" s="8" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
@@ -661,12 +660,12 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
-      <c r="C7" s="9">
+      <c r="C7" s="5">
         <v>45802</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
       <c r="H7" s="1" t="s">
         <v>4</v>
       </c>
@@ -783,12 +782,12 @@
       <c r="F11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="13"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="12"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
@@ -810,7 +809,7 @@
       <c r="I12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K12" s="4"/>
@@ -835,7 +834,7 @@
       <c r="I13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K13" s="4"/>
@@ -896,22 +895,22 @@
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
-      <c r="C16" s="9">
+      <c r="C16" s="5">
         <v>45802</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
       <c r="H16" s="2" t="s">
         <v>4</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J16" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K16" s="10" t="s">
+      <c r="J16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -933,10 +932,10 @@
       <c r="I17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J17" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K17" s="10" t="s">
+      <c r="J17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -967,12 +966,12 @@
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
-      <c r="C19" s="9">
+      <c r="C19" s="5">
         <v>45809</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
       <c r="H19" s="2" t="s">
         <v>1</v>
       </c>
@@ -1002,7 +1001,7 @@
       <c r="I20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K20" s="4"/>
@@ -1023,7 +1022,7 @@
       <c r="I21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J21" s="10" t="s">
+      <c r="J21" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K21" s="4"/>
@@ -1044,7 +1043,7 @@
       <c r="I22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J22" s="10" t="s">
+      <c r="J22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K22" s="4"/>
@@ -1065,7 +1064,7 @@
       <c r="I23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J23" s="10" t="s">
+      <c r="J23" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K23" s="4"/>
@@ -1086,7 +1085,7 @@
       <c r="I24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J24" s="10" t="s">
+      <c r="J24" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K24" s="4"/>
@@ -1107,7 +1106,7 @@
       <c r="I25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="10" t="s">
+      <c r="J25" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K25" s="4"/>
@@ -1128,7 +1127,7 @@
       <c r="I26" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J26" s="10" t="s">
+      <c r="J26" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K26" s="4"/>
@@ -1151,10 +1150,10 @@
       <c r="I27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J27" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K27" s="10" t="s">
+      <c r="J27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1176,25 +1175,25 @@
       <c r="I28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J28" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K28" s="10" t="s">
+      <c r="J28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K28" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
-      <c r="C29" s="5">
+      <c r="C29" s="6">
         <v>45814</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="7"/>
-      <c r="H29" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="I29" s="10" t="s">
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="8"/>
+      <c r="H29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J29" s="2" t="s">
@@ -1245,12 +1244,12 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
-      <c r="C33" s="5">
+      <c r="C33" s="6">
         <v>45814</v>
       </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="8"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
@@ -1322,12 +1321,12 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
-      <c r="C38" s="9">
+      <c r="C38" s="5">
         <v>45814</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
@@ -1383,12 +1382,12 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
-      <c r="C43" s="9">
+      <c r="C43" s="5">
         <v>45830</v>
       </c>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
@@ -1561,12 +1560,12 @@
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
-      <c r="C57" s="9">
+      <c r="C57" s="5">
         <v>45835</v>
       </c>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="3">
@@ -1726,12 +1725,12 @@
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
-      <c r="C70" s="9">
+      <c r="C70" s="5">
         <v>45838</v>
       </c>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
-      <c r="F70" s="9"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="3">
@@ -1826,12 +1825,12 @@
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="3"/>
-      <c r="C78" s="9">
+      <c r="C78" s="5">
         <v>45838</v>
       </c>
-      <c r="D78" s="9"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" s="3">
@@ -1903,11 +1902,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C78:F78"/>
-    <mergeCell ref="C70:F70"/>
     <mergeCell ref="C33:F33"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="C2:F2"/>
@@ -1916,6 +1910,11 @@
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C29:F29"/>
     <mergeCell ref="H11:K11"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C78:F78"/>
+    <mergeCell ref="C70:F70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Improved visuals for Player Profile Page, yet to be further enhancements
</commit_message>
<xml_diff>
--- a/List.xlsx
+++ b/List.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\VSCode Projects\pool-cost-calculator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\VSCode_Projects\pool-cost-calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AE8871-A2AC-4FA5-A704-31DBA091D80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D198E4B3-D0A3-4DF8-AC7C-EEC340DF58D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-7215" windowWidth="16440" windowHeight="28320" xr2:uid="{BE88EEF3-4FF8-43A6-B5B5-5525606DC647}"/>
+    <workbookView xWindow="-16320" yWindow="-7215" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{BE88EEF3-4FF8-43A6-B5B5-5525606DC647}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="14">
   <si>
     <t>H</t>
   </si>
@@ -63,6 +64,21 @@
   </si>
   <si>
     <t>Test2</t>
+  </si>
+  <si>
+    <t>Wilbert</t>
+  </si>
+  <si>
+    <t>Isaac</t>
+  </si>
+  <si>
+    <t>Eden</t>
+  </si>
+  <si>
+    <t>Li Sheng</t>
+  </si>
+  <si>
+    <t>Henry</t>
   </si>
 </sst>
 </file>
@@ -170,9 +186,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -183,6 +196,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -528,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9C6144-6401-498D-8D34-6B35F906CB82}">
-  <dimension ref="B2:K82"/>
+  <dimension ref="B2:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,22 +555,16 @@
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="5">
+      <c r="C2" s="9">
         <v>45795</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="H2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>1</v>
       </c>
@@ -570,16 +580,8 @@
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -595,16 +597,8 @@
       <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -620,16 +614,8 @@
       <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>4</v>
       </c>
@@ -645,41 +631,17 @@
       <c r="F6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
-      <c r="C7" s="5">
+      <c r="C7" s="9">
         <v>45802</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="H7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>1</v>
       </c>
@@ -695,20 +657,8 @@
       <c r="F8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>2</v>
       </c>
@@ -724,20 +674,8 @@
       <c r="F9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>3</v>
       </c>
@@ -753,20 +691,8 @@
       <c r="F10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>4</v>
       </c>
@@ -782,14 +708,8 @@
       <c r="F11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="12"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>5</v>
       </c>
@@ -805,16 +725,8 @@
       <c r="F12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>6</v>
       </c>
@@ -830,16 +742,8 @@
       <c r="F13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>7</v>
       </c>
@@ -855,16 +759,8 @@
       <c r="F14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>8</v>
       </c>
@@ -880,41 +776,17 @@
       <c r="F15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
-      <c r="C16" s="5">
+      <c r="C16" s="9">
         <v>45802</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="H16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>1</v>
       </c>
@@ -926,20 +798,8 @@
         <v>2</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="H17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <v>2</v>
       </c>
@@ -951,41 +811,17 @@
         <v>5</v>
       </c>
       <c r="F18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
-      <c r="C19" s="5">
+      <c r="C19" s="9">
         <v>45809</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="H19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>1</v>
       </c>
@@ -997,16 +833,8 @@
         <v>0</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <v>2</v>
       </c>
@@ -1018,16 +846,8 @@
         <v>0</v>
       </c>
       <c r="F21" s="1"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K21" s="4"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>3</v>
       </c>
@@ -1039,16 +859,8 @@
         <v>0</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <v>4</v>
       </c>
@@ -1060,16 +872,8 @@
         <v>6</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K23" s="4"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <v>5</v>
       </c>
@@ -1081,16 +885,8 @@
         <v>0</v>
       </c>
       <c r="F24" s="1"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K24" s="4"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <v>6</v>
       </c>
@@ -1102,16 +898,8 @@
         <v>6</v>
       </c>
       <c r="F25" s="1"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K25" s="4"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <v>7</v>
       </c>
@@ -1123,16 +911,8 @@
         <v>0</v>
       </c>
       <c r="F26" s="1"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K26" s="4"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <v>8</v>
       </c>
@@ -1144,20 +924,8 @@
         <v>6</v>
       </c>
       <c r="F27" s="1"/>
-      <c r="H27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <v>9</v>
       </c>
@@ -1169,41 +937,17 @@
         <v>6</v>
       </c>
       <c r="F28" s="1"/>
-      <c r="H28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
-      <c r="C29" s="6">
+      <c r="C29" s="5">
         <v>45814</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="8"/>
-      <c r="H29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <v>1</v>
       </c>
@@ -1216,7 +960,7 @@
       </c>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
         <v>2</v>
       </c>
@@ -1229,7 +973,7 @@
       </c>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
         <v>3</v>
       </c>
@@ -1244,12 +988,12 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
-      <c r="C33" s="6">
+      <c r="C33" s="5">
         <v>45814</v>
       </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="8"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="7"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
@@ -1321,12 +1065,12 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
-      <c r="C38" s="5">
+      <c r="C38" s="9">
         <v>45814</v>
       </c>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
@@ -1382,12 +1126,12 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
-      <c r="C43" s="5">
+      <c r="C43" s="9">
         <v>45830</v>
       </c>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
@@ -1560,12 +1304,12 @@
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
-      <c r="C57" s="5">
+      <c r="C57" s="9">
         <v>45835</v>
       </c>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="3">
@@ -1725,12 +1469,12 @@
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
-      <c r="C70" s="5">
+      <c r="C70" s="9">
         <v>45838</v>
       </c>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="3">
@@ -1825,12 +1569,12 @@
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="3"/>
-      <c r="C78" s="5">
+      <c r="C78" s="9">
         <v>45838</v>
       </c>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" s="3">
@@ -1901,20 +1645,365 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="11">
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C78:F78"/>
+    <mergeCell ref="C70:F70"/>
     <mergeCell ref="C33:F33"/>
-    <mergeCell ref="H2:K2"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C29:F29"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C78:F78"/>
-    <mergeCell ref="C70:F70"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27B7492-A177-42CB-A550-71B20340A114}">
+  <dimension ref="B2:E29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Recent Matches table to view latest matches on main page
</commit_message>
<xml_diff>
--- a/List.xlsx
+++ b/List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\VSCode_Projects\pool-cost-calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D198E4B3-D0A3-4DF8-AC7C-EEC340DF58D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39CE7F0-2630-4ABA-962F-A94130D4132C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-7215" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{BE88EEF3-4FF8-43A6-B5B5-5525606DC647}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="15">
   <si>
     <t>H</t>
   </si>
@@ -60,9 +60,6 @@
     <t>K</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>Test2</t>
   </si>
   <si>
@@ -79,6 +76,12 @@
   </si>
   <si>
     <t>Henry</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>Test1</t>
   </si>
 </sst>
 </file>
@@ -114,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -174,18 +177,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -196,20 +214,51 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,7 +596,7 @@
   <dimension ref="B2:F82"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,12 +606,12 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="9">
+      <c r="C2" s="4">
         <v>45795</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
@@ -634,12 +683,12 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
-      <c r="C7" s="9">
+      <c r="C7" s="4">
         <v>45802</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
@@ -779,12 +828,12 @@
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
-      <c r="C16" s="9">
+      <c r="C16" s="4">
         <v>45802</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
@@ -814,12 +863,12 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
-      <c r="C19" s="9">
+      <c r="C19" s="4">
         <v>45809</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
@@ -1065,12 +1114,12 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
-      <c r="C38" s="9">
+      <c r="C38" s="4">
         <v>45814</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
@@ -1126,12 +1175,12 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
-      <c r="C43" s="9">
+      <c r="C43" s="4">
         <v>45830</v>
       </c>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
@@ -1304,12 +1353,12 @@
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
-      <c r="C57" s="9">
+      <c r="C57" s="4">
         <v>45835</v>
       </c>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="3">
@@ -1469,12 +1518,12 @@
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
-      <c r="C70" s="9">
+      <c r="C70" s="4">
         <v>45838</v>
       </c>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
-      <c r="F70" s="9"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="3">
@@ -1569,12 +1618,12 @@
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="3"/>
-      <c r="C78" s="9">
+      <c r="C78" s="4">
         <v>45838</v>
       </c>
-      <c r="D78" s="9"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" s="3">
@@ -1646,17 +1695,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C78:F78"/>
-    <mergeCell ref="C70:F70"/>
     <mergeCell ref="C33:F33"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C78:F78"/>
+    <mergeCell ref="C70:F70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1664,346 +1713,589 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27B7492-A177-42CB-A550-71B20340A114}">
-  <dimension ref="B2:E29"/>
+  <dimension ref="A2:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="4"/>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="18"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="18"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="18"/>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="18"/>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="18"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="12"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="12"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="C13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="4"/>
-      <c r="C21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
-      <c r="C22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
-      <c r="C23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
-      <c r="C24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
-      <c r="C25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-      <c r="C26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>5</v>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>0</v>
+      </c>
+      <c r="B31" s="23"/>
+      <c r="C31" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="23"/>
+      <c r="F31" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>0</v>
+      </c>
+      <c r="B32" s="23"/>
+      <c r="C32" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="23"/>
+      <c r="F32" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
+        <v>4</v>
+      </c>
+      <c r="B33" s="23"/>
+      <c r="C33" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="23"/>
+      <c r="F33" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
+        <v>0</v>
+      </c>
+      <c r="B34" s="23"/>
+      <c r="C34" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="23"/>
+      <c r="F34" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="8">
+        <v>0</v>
+      </c>
+      <c r="B35" s="23"/>
+      <c r="C35" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="23"/>
+      <c r="F35" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
+        <v>7</v>
+      </c>
+      <c r="B36" s="23"/>
+      <c r="C36" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="23"/>
+      <c r="F36" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="9">
+        <v>0</v>
+      </c>
+      <c r="B37" s="23"/>
+      <c r="C37" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="23"/>
+      <c r="F37" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
+        <v>0</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="8">
+        <v>0</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="8">
+        <v>0</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="10">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B30:E30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Admin page and moved clear all data to Admin page
</commit_message>
<xml_diff>
--- a/List.xlsx
+++ b/List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\VSCode_Projects\pool-cost-calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39CE7F0-2630-4ABA-962F-A94130D4132C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C578841-3F7C-47C3-9821-35813B60B86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-7215" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{BE88EEF3-4FF8-43A6-B5B5-5525606DC647}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="16">
   <si>
     <t>H</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Test1</t>
+  </si>
+  <si>
+    <t>Test4</t>
   </si>
 </sst>
 </file>
@@ -194,24 +197,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -228,6 +219,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -243,22 +259,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,12 +619,12 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="4">
+      <c r="C2" s="17">
         <v>45795</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
@@ -683,12 +696,12 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
-      <c r="C7" s="4">
+      <c r="C7" s="17">
         <v>45802</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
@@ -828,12 +841,12 @@
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
-      <c r="C16" s="4">
+      <c r="C16" s="17">
         <v>45802</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
@@ -863,12 +876,12 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
-      <c r="C19" s="4">
+      <c r="C19" s="17">
         <v>45809</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
@@ -989,12 +1002,12 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
-      <c r="C29" s="5">
+      <c r="C29" s="14">
         <v>45814</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="7"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="16"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
@@ -1037,12 +1050,12 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
-      <c r="C33" s="5">
+      <c r="C33" s="14">
         <v>45814</v>
       </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="7"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="16"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
@@ -1114,12 +1127,12 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
-      <c r="C38" s="4">
+      <c r="C38" s="17">
         <v>45814</v>
       </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
@@ -1175,12 +1188,12 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
-      <c r="C43" s="4">
+      <c r="C43" s="17">
         <v>45830</v>
       </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
@@ -1353,12 +1366,12 @@
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
-      <c r="C57" s="4">
+      <c r="C57" s="17">
         <v>45835</v>
       </c>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="3">
@@ -1518,12 +1531,12 @@
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
-      <c r="C70" s="4">
+      <c r="C70" s="17">
         <v>45838</v>
       </c>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
+      <c r="F70" s="17"/>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="3">
@@ -1618,12 +1631,12 @@
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="3"/>
-      <c r="C78" s="4">
+      <c r="C78" s="17">
         <v>45838</v>
       </c>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" s="3">
@@ -1695,17 +1708,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C78:F78"/>
+    <mergeCell ref="C70:F70"/>
     <mergeCell ref="C33:F33"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C78:F78"/>
-    <mergeCell ref="C70:F70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1713,10 +1726,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27B7492-A177-42CB-A550-71B20340A114}">
-  <dimension ref="A2:F40"/>
+  <dimension ref="A2:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,57 +1739,57 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="12"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="18"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="12"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="18"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="12"/>
+      <c r="D4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="12"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="19" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1785,62 +1798,62 @@
       <c r="E6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="12"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="19" t="s">
+      <c r="D7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="12"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="12"/>
+      <c r="D8" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="12"/>
+      <c r="D9" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="19" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -1849,60 +1862,60 @@
       <c r="E10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="12"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="14" t="s">
+      <c r="A11" s="8"/>
+      <c r="B11" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="12"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19" t="s">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="12"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19" t="s">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="12"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19" t="s">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="12"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="19" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -1911,14 +1924,14 @@
       <c r="E15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="12"/>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="19" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1927,14 +1940,14 @@
       <c r="E16" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F16" s="12"/>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="19" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1943,30 +1956,30 @@
       <c r="E17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F17" s="12"/>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="F18" s="12"/>
+      <c r="D18" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="19" t="s">
+      <c r="A19" s="8"/>
+      <c r="B19" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -1975,98 +1988,98 @@
       <c r="E19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="12"/>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="12"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="12"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19" t="s">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="12"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19" t="s">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="12"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19" t="s">
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="12"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19" t="s">
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="12"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19" t="s">
+      <c r="A26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E26" s="18"/>
-      <c r="F26" s="12"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="19" t="s">
+      <c r="A27" s="8"/>
+      <c r="B27" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -2075,14 +2088,14 @@
       <c r="E27" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="12"/>
+      <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="19" t="s">
+      <c r="A28" s="8"/>
+      <c r="B28" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D28" s="3" t="s">
@@ -2091,211 +2104,264 @@
       <c r="E28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="12"/>
+      <c r="F28" s="8"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
+      <c r="A29" s="8"/>
       <c r="B29" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F29" s="12"/>
+      <c r="D29" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="8"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="17" t="s">
+      <c r="A30" s="8"/>
+      <c r="B30" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="12"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
-        <v>0</v>
-      </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="E31" s="23"/>
-      <c r="F31" s="10">
+      <c r="A31" s="4">
+        <v>0</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
-        <v>0</v>
-      </c>
-      <c r="B32" s="23"/>
-      <c r="C32" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="10">
+      <c r="A32" s="4">
+        <v>0</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
-        <v>4</v>
-      </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="23"/>
-      <c r="F33" s="10">
+      <c r="A33" s="4">
+        <v>4</v>
+      </c>
+      <c r="B33" s="13"/>
+      <c r="C33" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
-        <v>0</v>
-      </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E34" s="23"/>
-      <c r="F34" s="10">
+      <c r="A34" s="4">
+        <v>0</v>
+      </c>
+      <c r="B34" s="13"/>
+      <c r="C34" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="13"/>
+      <c r="F34" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="8">
-        <v>0</v>
-      </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="10">
+      <c r="A35" s="4">
+        <v>0</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="8">
+      <c r="A36" s="4">
         <v>7</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="10">
+      <c r="B36" s="13"/>
+      <c r="C36" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
-        <v>0</v>
-      </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="11">
+      <c r="A37" s="5">
+        <v>0</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="13"/>
+      <c r="F37" s="7">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
-        <v>0</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E38" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="F38" s="10">
-        <v>5</v>
-      </c>
+      <c r="A38" s="26"/>
+      <c r="B38" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="25"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="8">
-        <v>0</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="F39" s="10">
+      <c r="A39" s="4">
+        <v>0</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="8">
-        <v>0</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="F40" s="10">
-        <v>3</v>
+      <c r="A40" s="26"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="9"/>
+      <c r="F40" s="25"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="24"/>
+      <c r="C41" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="24"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="24"/>
+      <c r="C42" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="24"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>0</v>
+      </c>
+      <c r="B44" s="24"/>
+      <c r="C44" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="24"/>
+      <c r="F44" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>0</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F45" s="27">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B43:E43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed winrate bugs, refined aesthetics of table
</commit_message>
<xml_diff>
--- a/List.xlsx
+++ b/List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\VSCode_Projects\pool-cost-calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C578841-3F7C-47C3-9821-35813B60B86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18604D0B-CB01-4400-B97A-31EA9321F1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-7215" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{BE88EEF3-4FF8-43A6-B5B5-5525606DC647}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="64">
   <si>
     <t>H</t>
   </si>
@@ -85,6 +85,150 @@
   </si>
   <si>
     <t>Test4</t>
+  </si>
+  <si>
+    <t>N [8]</t>
+  </si>
+  <si>
+    <t>I (0)</t>
+  </si>
+  <si>
+    <t>LS (2)</t>
+  </si>
+  <si>
+    <t>N (1)</t>
+  </si>
+  <si>
+    <t>LS (0)</t>
+  </si>
+  <si>
+    <t>N (3)</t>
+  </si>
+  <si>
+    <t>I (1)</t>
+  </si>
+  <si>
+    <t>LS (0) [8]</t>
+  </si>
+  <si>
+    <t>I [8]</t>
+  </si>
+  <si>
+    <t>N (4)</t>
+  </si>
+  <si>
+    <t>I (0) [8]</t>
+  </si>
+  <si>
+    <t>N (2)</t>
+  </si>
+  <si>
+    <t>LS (3)</t>
+  </si>
+  <si>
+    <t>N (6)</t>
+  </si>
+  <si>
+    <t>I + E</t>
+  </si>
+  <si>
+    <t>(1) [8]</t>
+  </si>
+  <si>
+    <t>(2)</t>
+  </si>
+  <si>
+    <t>(0)</t>
+  </si>
+  <si>
+    <t>N + LS</t>
+  </si>
+  <si>
+    <t>(1)</t>
+  </si>
+  <si>
+    <t>()</t>
+  </si>
+  <si>
+    <t>balls left</t>
+  </si>
+  <si>
+    <t>[8]</t>
+  </si>
+  <si>
+    <t>8 Ball Scratch</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>Faults</t>
+  </si>
+  <si>
+    <t>LS (0) {1}</t>
+  </si>
+  <si>
+    <t>H (3) {1}</t>
+  </si>
+  <si>
+    <t>LS (2) {1}</t>
+  </si>
+  <si>
+    <t>I (0) {0}</t>
+  </si>
+  <si>
+    <t>I (0) {3} [8]</t>
+  </si>
+  <si>
+    <t>H (1) {3}</t>
+  </si>
+  <si>
+    <t>H (1) {2}</t>
+  </si>
+  <si>
+    <t>LS (0) {0}</t>
+  </si>
+  <si>
+    <t>I (1) {2}</t>
+  </si>
+  <si>
+    <t>LS (0) {2}</t>
+  </si>
+  <si>
+    <t>H (0) {4}</t>
+  </si>
+  <si>
+    <t>LS (1) {0}</t>
+  </si>
+  <si>
+    <t>I (0) {1}</t>
+  </si>
+  <si>
+    <t>H (0) {2}</t>
+  </si>
+  <si>
+    <t>I (0) {3}</t>
+  </si>
+  <si>
+    <t>I (3) {3}</t>
+  </si>
+  <si>
+    <t>LS (0) {2} [8]</t>
+  </si>
+  <si>
+    <t>I (2) {3}</t>
+  </si>
+  <si>
+    <t>H (4) {2} [8]</t>
+  </si>
+  <si>
+    <t>1v1</t>
+  </si>
+  <si>
+    <t>2v2</t>
+  </si>
+  <si>
+    <t>Overall</t>
   </si>
 </sst>
 </file>
@@ -197,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -232,6 +376,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -239,9 +396,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -256,21 +410,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -606,25 +750,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9C6144-6401-498D-8D34-6B35F906CB82}">
-  <dimension ref="B2:F82"/>
+  <dimension ref="B2:I93"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="17">
+      <c r="C2" s="18">
         <v>45795</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
@@ -696,12 +840,12 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
-      <c r="C7" s="17">
+      <c r="C7" s="18">
         <v>45802</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
@@ -841,12 +985,12 @@
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
-      <c r="C16" s="17">
+      <c r="C16" s="18">
         <v>45802</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
@@ -876,12 +1020,12 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
-      <c r="C19" s="17">
+      <c r="C19" s="18">
         <v>45809</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
@@ -1002,12 +1146,12 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
-      <c r="C29" s="14">
+      <c r="C29" s="19">
         <v>45814</v>
       </c>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="16"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="21"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
@@ -1050,12 +1194,12 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
-      <c r="C33" s="14">
+      <c r="C33" s="19">
         <v>45814</v>
       </c>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="16"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="21"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
@@ -1127,12 +1271,12 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
-      <c r="C38" s="17">
+      <c r="C38" s="18">
         <v>45814</v>
       </c>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
@@ -1188,12 +1332,12 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
-      <c r="C43" s="17">
+      <c r="C43" s="18">
         <v>45830</v>
       </c>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
@@ -1230,7 +1374,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="F46" s="1"/>
     </row>
@@ -1366,12 +1510,12 @@
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
-      <c r="C57" s="17">
+      <c r="C57" s="18">
         <v>45835</v>
       </c>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="3">
@@ -1382,7 +1526,7 @@
         <v>2</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F58" s="1"/>
     </row>
@@ -1418,10 +1562,10 @@
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F61" s="1"/>
     </row>
@@ -1431,10 +1575,10 @@
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F62" s="1"/>
     </row>
@@ -1444,10 +1588,10 @@
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F63" s="1"/>
     </row>
@@ -1457,27 +1601,27 @@
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="3">
         <v>8</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="3">
         <v>9</v>
       </c>
@@ -1490,7 +1634,7 @@
       </c>
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="3">
         <v>10</v>
       </c>
@@ -1503,233 +1647,394 @@
       </c>
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="3">
         <v>11</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="3">
         <v>12</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="2" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
-      <c r="C70" s="17">
+      <c r="C70" s="18">
         <v>45838</v>
       </c>
-      <c r="D70" s="17"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="17"/>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="3">
         <v>1</v>
       </c>
       <c r="C71" s="1"/>
-      <c r="D71" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>5</v>
+      <c r="D71" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E71" s="26" t="s">
+        <v>19</v>
       </c>
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="3">
         <v>2</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="3">
         <v>3</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="3">
         <v>4</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="3">
         <v>5</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="3">
         <v>6</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="3">
         <v>7</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="2" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="3"/>
-      <c r="C78" s="17">
+      <c r="C78" s="18">
         <v>45838</v>
       </c>
-      <c r="D78" s="17"/>
-      <c r="E78" s="17"/>
-      <c r="F78" s="17"/>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D78" s="18"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="3">
         <v>1</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="D79" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E79" s="28" t="s">
+        <v>33</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="H79" t="s">
+        <v>36</v>
+      </c>
+      <c r="I79" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="3">
         <v>2</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="D80" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E80" s="27" t="s">
+        <v>35</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="H80" t="s">
+        <v>38</v>
+      </c>
+      <c r="I80" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="3">
         <v>3</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="D81" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E81" s="27" t="s">
+        <v>32</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="H81" t="s">
+        <v>40</v>
+      </c>
+      <c r="I81" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="3">
         <v>4</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="D82" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E82" s="28" t="s">
+        <v>33</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>1</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="1"/>
+      <c r="C83" s="18">
+        <v>45857</v>
+      </c>
+      <c r="D83" s="18"/>
+      <c r="E83" s="18"/>
+      <c r="F83" s="18"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B84" s="29">
+        <v>1</v>
+      </c>
+      <c r="C84" s="1"/>
+      <c r="D84" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F84" s="1"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B85" s="29">
+        <v>2</v>
+      </c>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F85" s="1"/>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B86" s="29">
+        <v>3</v>
+      </c>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F86" s="1"/>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B87" s="29">
+        <v>4</v>
+      </c>
+      <c r="C87" s="1"/>
+      <c r="D87" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F87" s="1"/>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B88" s="29">
+        <v>5</v>
+      </c>
+      <c r="C88" s="1"/>
+      <c r="D88" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F88" s="1"/>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B89" s="29">
+        <v>6</v>
+      </c>
+      <c r="C89" s="1"/>
+      <c r="D89" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F89" s="1"/>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="29">
+        <v>7</v>
+      </c>
+      <c r="C90" s="1"/>
+      <c r="D90" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F90" s="1"/>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B91" s="29">
+        <v>8</v>
+      </c>
+      <c r="C91" s="1"/>
+      <c r="D91" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F91" s="1"/>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B92" s="29">
+        <v>9</v>
+      </c>
+      <c r="C92" s="1"/>
+      <c r="D92" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F92" s="1"/>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B93" s="29">
+        <v>10</v>
+      </c>
+      <c r="C93" s="1"/>
+      <c r="D93" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F93" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C78:F78"/>
-    <mergeCell ref="C70:F70"/>
+  <mergeCells count="12">
+    <mergeCell ref="C83:F83"/>
     <mergeCell ref="C33:F33"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C78:F78"/>
+    <mergeCell ref="C70:F70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D79:D81 E79:E82" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27B7492-A177-42CB-A550-71B20340A114}">
-  <dimension ref="A2:F45"/>
+  <dimension ref="A2:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,17 +2043,17 @@
     <col min="6" max="6" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="9"/>
       <c r="C3" s="3" t="s">
@@ -1759,8 +2064,15 @@
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
       <c r="C4" s="3" t="s">
@@ -1771,8 +2083,18 @@
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4">
+        <f>2/5</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
@@ -1783,8 +2105,15 @@
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5">
+        <f>4/8</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="10" t="s">
         <v>1</v>
@@ -1799,8 +2128,15 @@
         <v>3</v>
       </c>
       <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6">
+        <f>1/1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="3" t="s">
         <v>4</v>
@@ -1815,8 +2151,18 @@
         <v>12</v>
       </c>
       <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="3" t="s">
         <v>3</v>
@@ -1831,8 +2177,15 @@
         <v>0</v>
       </c>
       <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8">
+        <f>6/6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="3" t="s">
         <v>3</v>
@@ -1847,8 +2200,14 @@
         <v>0</v>
       </c>
       <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="10" t="s">
         <v>1</v>
@@ -1863,18 +2222,35 @@
         <v>4</v>
       </c>
       <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10">
+        <f>3/4</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25"/>
       <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J11">
+        <f>3/4</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="10" t="s">
@@ -1885,8 +2261,15 @@
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12">
+        <f>0/1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10" t="s">
@@ -1897,8 +2280,18 @@
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13">
+        <f>0/3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10" t="s">
@@ -1909,8 +2302,15 @@
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14">
+        <f>0/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="10" t="s">
         <v>1</v>
@@ -1925,8 +2325,15 @@
         <v>3</v>
       </c>
       <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15">
+        <f>0/1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="10" t="s">
         <v>4</v>
@@ -1941,8 +2348,18 @@
         <v>0</v>
       </c>
       <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J16">
+        <f>0/3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="10" t="s">
         <v>3</v>
@@ -1957,8 +2374,15 @@
         <v>0</v>
       </c>
       <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17">
+        <f>0/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="3" t="s">
         <v>3</v>
@@ -1974,7 +2398,7 @@
       </c>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="10" t="s">
         <v>1</v>
@@ -1990,7 +2414,7 @@
       </c>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="10" t="s">
@@ -2002,7 +2426,7 @@
       <c r="E20" s="9"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="10" t="s">
@@ -2014,7 +2438,7 @@
       <c r="E21" s="9"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10" t="s">
@@ -2026,7 +2450,7 @@
       <c r="E22" s="9"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
       <c r="C23" s="10" t="s">
@@ -2038,7 +2462,7 @@
       <c r="E23" s="9"/>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10" t="s">
@@ -2050,7 +2474,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10" t="s">
@@ -2062,7 +2486,7 @@
       <c r="E25" s="9"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="10" t="s">
@@ -2074,7 +2498,7 @@
       <c r="E26" s="9"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="10" t="s">
         <v>4</v>
@@ -2090,7 +2514,7 @@
       </c>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="10" t="s">
         <v>4</v>
@@ -2106,7 +2530,7 @@
       </c>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="3" t="s">
         <v>4</v>
@@ -2122,17 +2546,17 @@
       </c>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>0</v>
       </c>
@@ -2148,7 +2572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>0</v>
       </c>
@@ -2245,7 +2669,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
+      <c r="A38" s="16"/>
       <c r="B38" s="10" t="s">
         <v>3</v>
       </c>
@@ -2258,7 +2682,7 @@
       <c r="E38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F38" s="25"/>
+      <c r="F38" s="15"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
@@ -2281,7 +2705,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
+      <c r="A40" s="16"/>
       <c r="B40" s="9"/>
       <c r="C40" s="10" t="s">
         <v>0</v>
@@ -2290,49 +2714,49 @@
         <v>3</v>
       </c>
       <c r="E40" s="9"/>
-      <c r="F40" s="25"/>
+      <c r="F40" s="15"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="24"/>
+      <c r="B41" s="14"/>
       <c r="C41" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="E41" s="24"/>
+      <c r="D41" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="14"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="24"/>
+      <c r="B42" s="14"/>
       <c r="C42" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D42" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="E42" s="24"/>
+      <c r="D42" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="14"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>0</v>
       </c>
-      <c r="B44" s="24"/>
+      <c r="B44" s="14"/>
       <c r="C44" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D44" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="27">
+      <c r="D44" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="14"/>
+      <c r="F44" s="17">
         <v>3</v>
       </c>
     </row>
@@ -2346,13 +2770,13 @@
       <c r="C45" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D45" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F45" s="27">
+      <c r="F45" s="17">
         <v>4</v>
       </c>
     </row>

</xml_diff>